<commit_message>
Book work, Chapter 8
</commit_message>
<xml_diff>
--- a/Work Log Template.xlsx
+++ b/Work Log Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repo\ISIT-322-Developing-Mobile-Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871574E1-87AE-4631-BCF6-1FF3B30A24FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8820C800-C252-479F-82A0-C11FBA903C96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-16290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24630" yWindow="-14355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>In Class Lab Exercise</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>Labs 4</t>
+  </si>
+  <si>
+    <t>ADA Compliance</t>
+  </si>
+  <si>
+    <t>Lessons Learned</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
@@ -127,7 +136,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +148,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -227,12 +242,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2884049A-816E-4C90-B00B-7E195DC02E6F}" name="Table1" displayName="Table1" ref="B2:D25" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="B2:D25" xr:uid="{5498F7FE-F847-48FF-BEDF-35E97F747022}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2884049A-816E-4C90-B00B-7E195DC02E6F}" name="Table1" displayName="Table1" ref="B2:F26" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B2:F26" xr:uid="{5498F7FE-F847-48FF-BEDF-35E97F747022}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{ABDEFB6A-23E8-490B-8BA3-31FDB8C966B2}" name="Assignment Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{E1FB43F5-1B65-45C1-AB26-4B96C8816E4F}" name="Time in hrs" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{5D478A5E-037D-4E8B-B9AA-631F435B6FFD}" name="Due Date" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{45F01347-8B7E-4F42-B541-623DFB522E7F}" name="Lessons Learned"/>
+    <tableColumn id="5" xr3:uid="{AB71985B-FB49-4636-816E-9D615912E4D2}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -501,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D25"/>
+  <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,10 +529,11 @@
     <col min="2" max="2" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
@@ -525,8 +543,14 @@
       <c r="D2" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
@@ -535,7 +559,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>18</v>
       </c>
@@ -544,7 +568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>17</v>
       </c>
@@ -553,7 +577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
@@ -562,7 +586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>15</v>
       </c>
@@ -571,7 +595,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
@@ -580,7 +604,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
@@ -589,7 +613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
@@ -598,7 +622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
@@ -607,7 +631,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
@@ -616,7 +640,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -625,7 +649,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>5</v>
       </c>
@@ -634,7 +658,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
@@ -643,7 +667,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
@@ -730,6 +754,15 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
@@ -738,6 +771,7 @@
     <sortCondition ref="D3"/>
   </sortState>
   <dataConsolidate/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>